<commit_message>
telnet + metric ospf + bgp policies
</commit_message>
<xml_diff>
--- a/code/Def_Root_AS.xlsx
+++ b/code/Def_Root_AS.xlsx
@@ -605,7 +605,7 @@
         <v>True</v>
       </c>
       <c r="G7" t="str">
-        <v>[[2,8,""]]</v>
+        <v>[[2,8,"","customer"]]</v>
       </c>
     </row>
     <row r="8">
@@ -628,7 +628,7 @@
         <v>True</v>
       </c>
       <c r="G8" t="str">
-        <v>[[2,9,""]]</v>
+        <v>[[2,9,"","peer"]]</v>
       </c>
     </row>
     <row r="9">
@@ -651,7 +651,7 @@
         <v>True</v>
       </c>
       <c r="G9" t="str">
-        <v>[[1,6,""]]</v>
+        <v>[[1,6,"","provider"]]</v>
       </c>
     </row>
     <row r="10">
@@ -674,7 +674,7 @@
         <v>True</v>
       </c>
       <c r="G10" t="str">
-        <v>[[1,7,""]]</v>
+        <v>[[1,7,"","peer"]]</v>
       </c>
     </row>
     <row r="11">
@@ -691,7 +691,7 @@
         <v>["GigabiteEthernet1/0","GigabiteEthernet2/0","GigabiteEthernet3/0","GigabiteEthernet4/0"]</v>
       </c>
       <c r="E11" t="str">
-        <v>[[8,""],[9,""],[11,""],[12,""]]</v>
+        <v>[[8,"",500],[9,""],[11,""],[12,"",10]]</v>
       </c>
       <c r="F11" t="str">
         <v>False</v>

</xml_diff>